<commit_message>
update figures manuscript + SI
</commit_message>
<xml_diff>
--- a/2011Data.xlsx
+++ b/2011Data.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rebeccaciez/Documents/GitHub/CAFEStandardsCostReview/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E477BC-09FC-964B-8A99-DA01DE895890}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12AA9C65-5917-DA4C-B24F-E42872852505}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2380" yWindow="600" windowWidth="21100" windowHeight="14060" xr2:uid="{28A13116-7E2E-F842-AEE5-78E34D0C2240}"/>
+    <workbookView xWindow="2380" yWindow="460" windowWidth="21100" windowHeight="14060" xr2:uid="{28A13116-7E2E-F842-AEE5-78E34D0C2240}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -673,9 +673,9 @@
   <dimension ref="A1:T41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
       <selection activeCell="A11" sqref="A11"/>
-      <selection pane="topRight" activeCell="T2" sqref="T2"/>
+      <selection pane="topRight" activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>